<commit_message>
upload classificate and save resume
</commit_message>
<xml_diff>
--- a/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
+++ b/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
@@ -1,88 +1,140 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\פרוייקט\GIT פרוייקט עם\ResumeApp_Api\ResumeApp-Api\ResumeApp-Api\my_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9225"/>
-  </bookViews>
-  <sheets>
-    <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9225" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="גיליון1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <x:si>
+    <x:t>Path</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Class</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\cchvyunf.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Attribute not found</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\d5ouwqns.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\r3o2xpk0.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\m5yekaku.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\51dmony1.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\arzx4tcq.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\wmeronsg.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\h3dpuj4q.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\lspan1np.docx</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="177"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Arial"/>
+      <x:family val="2"/>
+      <x:charset val="177"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="12"/>
+      <x:color theme="1"/>
+      <x:name val="Arial"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -347,28 +399,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40.625" customWidth="1"/>
-    <col min="2" max="2" width="47.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B6"/>
+  <x:sheetViews>
+    <x:sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <x:cols>
+    <x:col min="1" max="1" width="40.625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="47.75" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <x:c r="A5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
adding the employer part
</commit_message>
<xml_diff>
--- a/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
+++ b/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <x:si>
     <x:t>Path</x:t>
   </x:si>
@@ -61,6 +61,36 @@
   </x:si>
   <x:si>
     <x:t>my_files\lspan1np.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GraphicsAndDesign</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\f0dybxje.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>בס -- 0 --&gt; ד -- Attribute not found</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\awqiqrmr.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\2enid42m.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">בס -- 0 --&gt; ד -- 0 --&gt; קורות -- </x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\idpfilow.doc</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">בס -- 0 --&gt; ד -- </x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\kzyqscg2.doc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>בס -- Attribute not found</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -403,9 +433,11 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B6"/>
+  <x:dimension ref="A1:B10"/>
   <x:sheetViews>
-    <x:sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <x:sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A10" sqref="A10"/>
+    </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <x:cols>
@@ -461,7 +493,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:2">
+    <x:row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A7" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
@@ -469,7 +501,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:2">
+    <x:row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A8" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -477,7 +509,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:2">
+    <x:row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A9" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -485,12 +517,52 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:2">
+    <x:row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A10" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:2">
+      <x:c r="A14" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:2">
+      <x:c r="A15" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
sending list of files
</commit_message>
<xml_diff>
--- a/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
+++ b/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
@@ -25,24 +25,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <x:si>
-    <x:t>Path</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Class</x:t>
-  </x:si>
-  <x:si>
-    <x:t>my_files\שירה אלנקוה - הנדסאי תכנה .pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>בתקשורת -- 0 --&gt; תכנון -- 0 --&gt; ב -- 0 --&gt; לב -- 0 --&gt; עיצוב -- 1 --&gt; GRAPHICSANDDESIG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>my_files\קורות חיים מיכל לאער.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>בתקשורת -- 0 --&gt; תכנון -- 0 --&gt; ב -- 1 --&gt; לידה -- 0 --&gt; מקצועית -- 0 --&gt; ARCHITECTUR</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <x:si>
+    <x:t>file.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COMPPROGRAMIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קוח-שירות-לקוחות.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OFFICEMANAGEMEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים מיכל לאער.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים אורי עוז מרזם.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARCHITECTUR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים מעודכן 2021.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ACCOUNTIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קוח-לדוגמא-מזכירות (1).pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>שירה טוויג.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים רחל רונס (1).pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים  פניני הוקס 0534106650.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GRAPHICSANDDESIG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CVשירה ג'יקובס  .pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>אבוחצירא.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים ברוריה רבינו.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>שירה אלנקוה - הנדסאי תכנה .pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים הדר המגיד 2021.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים לאה דנקור.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים לדוגמה למשרת הייטק.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים מרים ברודסקי.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים רחל בלעך.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>שירה בן תקוה הנדסאי תכנה (1) (1).pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>אילה קוח חדש.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EDUCATIO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>בתקשורת -- 0 --&gt; תכנון -- 0 --&gt; ב -- 0 --&gt; לב -- 0 --&gt; עיצוב -- 0 --&gt; ACCOUNTIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>בתקשורת -- 0 --&gt; תכנון -- 0 --&gt; ב -- 1 --&gt; לידה -- 1 --&gt; EDUCATIO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>קורות חיים אבי.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>בתקשורת -- 0 --&gt; תכנון -- 0 --&gt; ב -- 0 --&gt; לב -- 1 --&gt; בס -- 0 --&gt; ד -- 0 --&gt; קורות -- 0 --&gt; COMPPROGRAMING</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -52,21 +124,13 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="3" x14ac:knownFonts="1">
+  <x:fonts count="2" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Arial"/>
       <x:family val="2"/>
       <x:charset val="177"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:sz val="12"/>
-      <x:color theme="1"/>
-      <x:name val="Arial"/>
-      <x:family val="2"/>
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
@@ -77,12 +141,18 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFF00"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -96,13 +166,17 @@
   </x:borders>
   <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,27 +459,31 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B1"/>
+  <x:dimension ref="A1:B25"/>
   <x:sheetViews>
     <x:sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B12" sqref="B12"/>
+      <x:selection activeCell="A31" sqref="A31"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="1" width="40.625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="71.5" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="72" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="17" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="17.625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="20.375" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="39.875" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:2" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="1" t="s">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -413,12 +491,188 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2">
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A4" s="2" t="s">
         <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A8" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A9" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A12" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A14" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A15" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A16" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A17" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A18" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A19" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A20" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B20" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A21" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A22" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A23" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A24" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A25" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
working project before changeing model
</commit_message>
<xml_diff>
--- a/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
+++ b/ResumeApp-Api/ResumeApp-Api/my_files/DataBase.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <x:si>
     <x:t>file.pdf</x:t>
   </x:si>
@@ -115,6 +115,18 @@
   </x:si>
   <x:si>
     <x:t>בתקשורת -- 0 --&gt; תכנון -- 0 --&gt; ב -- 0 --&gt; לב -- 1 --&gt; בס -- 0 --&gt; ד -- 0 --&gt; קורות -- 0 --&gt; COMPPROGRAMING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\קורות חיים מיכל לאער (4).pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>בתקשורת -- 0 --&gt; תכנון -- 0 --&gt; ב -- 1 --&gt; לידה -- 0 --&gt; מקצועית -- 0 --&gt; ARCHITECTUR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\CVשירה ג'יקובס  .pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>my_files\קורות חיים אורי עוז מרזם.pdf</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -675,6 +687,30 @@
         <x:v>29</x:v>
       </x:c>
     </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>